<commit_message>
add a chart to the laporan_emas file
</commit_message>
<xml_diff>
--- a/emas.xlsx
+++ b/emas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-16 14:07:06</t>
+          <t>2025-12-19 14:59:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rp 23.200,00/ 0,01 gr</t>
+          <t>Rp 23.330,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rp 24.050,00/ 0,01 gr</t>
+          <t>Rp 24.180,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -478,12 +478,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-16 14:05:34</t>
+          <t>2025-12-19 14:54:33</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rp 23.200,00/ 0,01 gr</t>
+          <t>Rp 23.330,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rp 24.050,00/ 0,01 gr</t>
+          <t>Rp 24.180,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -505,12 +505,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-16 11:35:10</t>
+          <t>2025-12-18 14:13:46</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rp 23.250,00/ 0,01 gr</t>
+          <t>Rp 23.380,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rp 24.100,00/ 0,01 gr</t>
+          <t>Rp 24.230,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -532,12 +532,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-16 11:25:16</t>
+          <t>2025-12-18 13:50:18</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rp 23.250,00/ 0,01 gr</t>
+          <t>Rp 23.380,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Rp 24.100,00/ 0,01 gr</t>
+          <t>Rp 24.230,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -559,12 +559,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-16 11:24:15</t>
+          <t>2025-12-18 13:48:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rp 23.250,00/ 0,01 gr</t>
+          <t>Rp 23.380,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rp 24.100,00/ 0,01 gr</t>
+          <t>Rp 24.230,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -586,12 +586,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-16 11:16:13</t>
+          <t>2025-12-18 13:45:53</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rp 23.250,00/ 0,01 gr</t>
+          <t>Rp 23.380,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Rp 24.100,00/ 0,01 gr</t>
+          <t>Rp 24.230,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -613,12 +613,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-16 11:15:09</t>
+          <t>2025-12-18 13:45:50</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rp 23.250,00/ 0,01 gr</t>
+          <t>Rp 23.380,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rp 24.100,00/ 0,01 gr</t>
+          <t>Rp 24.230,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -640,12 +640,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-16 10:49:27</t>
+          <t>2025-12-18 13:42:40</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rp 23.250,00/ 0,01 gr</t>
+          <t>Rp 23.380,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rp 24.100,00/ 0,01 gr</t>
+          <t>Rp 24.230,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -667,12 +667,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-15 17:51:35</t>
+          <t>2025-12-18 11:49:33</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rp 23.200,00/ 0,01 gr</t>
+          <t>Rp 23.250,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Rp 24.050,00/ 0,01 gr</t>
+          <t>Rp 24.100,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -694,12 +694,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-15 14:54:27</t>
+          <t>2025-12-17 17:47:41</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rp 23.200,00/ 0,01 gr</t>
+          <t>Rp 23.250,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Rp 24.050,00/ 0,01 gr</t>
+          <t>Rp 24.100,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -721,12 +721,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-15 13:49:36</t>
+          <t>2025-12-17 17:06:24</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rp 23.200,00/ 0,01 gr</t>
+          <t>Rp 23.250,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Rp 24.050,00/ 0,01 gr</t>
+          <t>Rp 24.100,00/ 0,01 gr</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -748,25 +748,1051 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>2025-12-17 17:01:26</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-17 16:51:09</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-17 16:41:07</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-12-17 16:18:21</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-12-17 16:06:50</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:58:41</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:49:15</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:42:13</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:28:51</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-12-17 14:58:09</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-12-17 14:25:46</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-12-17 14:20:11</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:38:17</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:35:29</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:31:38</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>▲</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>▲</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-12-17 10:55:30</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-12-16 18:11:49</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:58:32</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:56:46</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:55:52</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:50:56</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:33:22</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:28:11</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:28:08</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:23:37</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:17:12</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:12:27</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-12-16 14:07:06</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-12-16 14:05:34</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>▼</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>▼</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:35:10</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:25:16</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:24:15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:16:13</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:15:09</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-12-16 10:49:27</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Rp 23.250,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>▲</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Rp 24.100,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>▲</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-12-15 17:51:35</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-12-15 14:54:27</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-12-15 13:49:36</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Rp 23.200,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Rp 24.050,00/ 0,01 gr</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>2025-12-15 12:51:25</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>Rp 23.200,00/ 0,01 gr</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
         <is>
           <t>Rp 24.050,00/ 0,01 gr</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>